<commit_message>
Removed email from vacation list. Moved it to the email list.
</commit_message>
<xml_diff>
--- a/matrixCompany2.xlsx
+++ b/matrixCompany2.xlsx
@@ -17,7 +17,7 @@
     <definedName function="false" hidden="false" name="BPOList" vbProcedure="false">'names and email'!#ref!</definedName>
     <definedName function="false" hidden="false" name="Domains" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Email" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">OnHoliday!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">OnHoliday!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Roles!$A$1:$K$9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Extract" vbProcedure="false">'Names and Email'!$B:$B</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Names and Email'!$A$1:$B$2</definedName>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
   <si>
     <t>Regular Approver</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Fill-In Approver</t>
   </si>
   <si>
-    <t>Fill-In Approver E-Mail Address</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>Approver FortyTwo</t>
   </si>
   <si>
-    <t>approver42@company2.com</t>
-  </si>
-  <si>
     <t>Role Name</t>
   </si>
   <si>
@@ -200,6 +194,9 @@
   </si>
   <si>
     <t>approver5@company2.com</t>
+  </si>
+  <si>
+    <t>approver42@company.com</t>
   </si>
 </sst>
 </file>
@@ -322,20 +319,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -428,25 +425,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -459,24 +456,19 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5" t="n">
+      <c r="C2" s="4" t="n">
         <v>42450</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="D2" s="4" t="n">
         <v>42731</v>
       </c>
     </row>
@@ -509,300 +501,300 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.7773279352227"/>
-    <col collapsed="false" hidden="false" max="10" min="5" style="1" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="1" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="7" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="I9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -822,80 +814,90 @@
     <tabColor rgb="FF000000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.9514170040486"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>

</xml_diff>